<commit_message>
Updated to write data from web page to excel sheet
</commit_message>
<xml_diff>
--- a/test/testdata/TestDataWrite.xlsx
+++ b/test/testdata/TestDataWrite.xlsx
@@ -4,6 +4,8 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Car" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -415,6 +417,54 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Ester</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Pantera</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Astor</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Linclon</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>age</v>
+      </c>
+      <c r="C1" t="str">
+        <v>car</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
         <v>tester</v>
       </c>
       <c r="B2">
@@ -424,9 +474,69 @@
         <v>sss</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>tester2</v>
+      </c>
+      <c r="B3">
+        <v>42</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Esteem</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>title</v>
+      </c>
+      <c r="B1" t="str">
+        <v>year</v>
+      </c>
+      <c r="C1" t="str">
+        <v>price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>location</v>
+      </c>
+      <c r="E1" t="str">
+        <v>phone</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>0714745050</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2014</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Rs 3,025,000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Avissawella,</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0714745050</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>